<commit_message>
Tests de performance con sockets en lan
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120718/Performance de nodo sockets.xlsx
+++ b/Documentacion/drafts/20120718/Performance de nodo sockets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Parametros de la VM</t>
   </si>
@@ -86,6 +86,30 @@
   </si>
   <si>
     <t>[200T-&gt;(kfgodel)-&gt;1R]</t>
+  </si>
+  <si>
+    <t>TestDePerformanceConNodoSocketsMismaLan</t>
+  </si>
+  <si>
+    <t>[1T-&gt;(wolfy)-&gt;1R]</t>
+  </si>
+  <si>
+    <t>[2T-&gt;(wolfy)-&gt;1R]</t>
+  </si>
+  <si>
+    <t>[4T-&gt;(wolfy)-&gt;1R]</t>
+  </si>
+  <si>
+    <t>[8T-&gt;(wolfy)-&gt;1R]</t>
+  </si>
+  <si>
+    <t>[16T-&gt;(wolfy)-&gt;1R]</t>
+  </si>
+  <si>
+    <t>[32T-&gt;(wolfy)-&gt;1R]</t>
+  </si>
+  <si>
+    <t>[200T-&gt;(wolfy)-&gt;1R]</t>
   </si>
 </sst>
 </file>
@@ -438,7 +462,7 @@
   <dimension ref="D2:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,58 +931,215 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="2">
+        <v>41107</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>10000</v>
+      </c>
+      <c r="F27" s="1">
+        <v>15.975199999999999</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.98019999999999996</v>
+      </c>
+      <c r="H27" s="3">
+        <f t="shared" ref="H27:H33" si="6">G27/F27</f>
+        <v>6.1357604286644302E-2</v>
+      </c>
+      <c r="I27" s="4">
+        <f>F27*1000</f>
+        <v>15975.199999999999</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" ref="J27:J33" si="7">G27*1000</f>
+        <v>980.19999999999993</v>
+      </c>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28">
+        <v>10000</v>
+      </c>
+      <c r="F28" s="1">
+        <v>16.666799999999999</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1.0943000000000001</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="6"/>
+        <v>6.5657474740202088E-2</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" ref="I28:I33" si="8">F28*1000</f>
+        <v>16666.8</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="7"/>
+        <v>1094.3</v>
+      </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>10000</v>
+      </c>
+      <c r="F29" s="1">
+        <v>17.142299999999999</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1.0909</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="6"/>
+        <v>6.36379015651342E-2</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="8"/>
+        <v>17142.3</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="7"/>
+        <v>1090.9000000000001</v>
+      </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <v>10016</v>
+      </c>
+      <c r="F30" s="1">
+        <v>16.459265175718802</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1.14007587859424</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="6"/>
+        <v>6.9266511379627929E-2</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" si="8"/>
+        <v>16459.265175718803</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="7"/>
+        <v>1140.0758785942401</v>
+      </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>10000</v>
+      </c>
+      <c r="F31" s="1">
+        <v>16.159199999999998</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1.1767000000000001</v>
+      </c>
+      <c r="H31" s="3">
+        <f t="shared" si="6"/>
+        <v>7.2819198970246066E-2</v>
+      </c>
+      <c r="I31" s="4">
+        <f t="shared" si="8"/>
+        <v>16159.199999999999</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="7"/>
+        <v>1176.7</v>
+      </c>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32">
+        <v>10000</v>
+      </c>
+      <c r="F32" s="1">
+        <v>15.631399999999999</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1.1367</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="6"/>
+        <v>7.2719014291746112E-2</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="8"/>
+        <v>15631.4</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="7"/>
+        <v>1136.7</v>
+      </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>10062</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4.1171735241502603</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1.27181474855893</v>
+      </c>
+      <c r="H33" s="3">
+        <f t="shared" si="6"/>
+        <v>0.30890482052767465</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="8"/>
+        <v>4117.1735241502602</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="7"/>
+        <v>1271.81474855893</v>
+      </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D36" s="2"/>
@@ -1174,7 +1355,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H7:H9 H13:H14">
-    <cfRule type="colorScale" priority="83">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1184,7 +1365,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="colorScale" priority="73">
+    <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1194,7 +1375,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="colorScale" priority="71">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1204,7 +1385,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="colorScale" priority="75">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1214,6 +1395,76 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37:H39 H43">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47:H49 H53">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H51">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -1223,18 +1474,118 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="H57:H59 H63">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67:H69 H73">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H72">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:H19 H23:H24">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1244,7 +1595,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H29 H33">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1254,7 +1605,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1264,7 +1615,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.9"/>
@@ -1274,176 +1625,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37:H39 H43">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H47:H49 H53">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H57:H59 H63">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H60">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67:H69 H73">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H71">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H19 H23:H24">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.9"/>
-        <color theme="5" tint="0.59999389629810485"/>
-        <color theme="6" tint="0.59999389629810485"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0.5"/>

</xml_diff>